<commit_message>
Excel files are now created for the input as well.
</commit_message>
<xml_diff>
--- a/input_excel.xlsx
+++ b/input_excel.xlsx
@@ -7,23 +7,23 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="iutmzejval" sheetId="1" r:id="rId1"/>
-    <sheet name="njocxezaks" sheetId="2" r:id="rId2"/>
-    <sheet name="krjyqnzsbl" sheetId="3" r:id="rId3"/>
-    <sheet name="jqlckxnreu" sheetId="4" r:id="rId4"/>
-    <sheet name="feqszgunji" sheetId="5" r:id="rId5"/>
-    <sheet name="qneajrzymv" sheetId="6" r:id="rId6"/>
-    <sheet name="hdxpefyvgc" sheetId="7" r:id="rId7"/>
-    <sheet name="vsqwnurcog" sheetId="8" r:id="rId8"/>
-    <sheet name="nagkxleity" sheetId="9" r:id="rId9"/>
-    <sheet name="aredwuqsjo" sheetId="10" r:id="rId10"/>
+    <sheet name="ibgwhcnkjd" sheetId="1" r:id="rId1"/>
+    <sheet name="mjugnarodb" sheetId="2" r:id="rId2"/>
+    <sheet name="bowxujcrqs" sheetId="3" r:id="rId3"/>
+    <sheet name="elxsivkfcn" sheetId="4" r:id="rId4"/>
+    <sheet name="qhrlazecip" sheetId="5" r:id="rId5"/>
+    <sheet name="jzcgoxqrbu" sheetId="6" r:id="rId6"/>
+    <sheet name="mqorxzhnfl" sheetId="7" r:id="rId7"/>
+    <sheet name="jbwsyquaox" sheetId="8" r:id="rId8"/>
+    <sheet name="fhcozyikgx" sheetId="9" r:id="rId9"/>
+    <sheet name="rqfuydwano" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="51">
   <si>
     <t>clientid</t>
   </si>
@@ -37,136 +37,145 @@
     <t>translationSetId</t>
   </si>
   <si>
-    <t>iutmzejval</t>
-  </si>
-  <si>
-    <t>['visual', 'gardens', 'cluster4']</t>
-  </si>
-  <si>
-    <t>1a918684-33d5-485a-80b7-90a8086803ef</t>
-  </si>
-  <si>
-    <t>f9d5d350-4bab-499a-8f53-2af1f6f25601</t>
-  </si>
-  <si>
-    <t>njocxezaks</t>
-  </si>
-  <si>
-    <t>['gardens', 'visual', 'cluster0']</t>
+    <t>ibgwhcnkjd</t>
+  </si>
+  <si>
+    <t>['cluster2', 'exhibition']</t>
+  </si>
+  <si>
+    <t>a42cba4d-03ab-449a-8fb5-a24fb363afa5</t>
+  </si>
+  <si>
+    <t>mjugnarodb</t>
+  </si>
+  <si>
+    <t>['parking', 'gardens']</t>
+  </si>
+  <si>
+    <t>7810d0eb-0034-457b-9cf7-ae7aa21e104f</t>
+  </si>
+  <si>
+    <t>bowxujcrqs</t>
+  </si>
+  <si>
+    <t>['cluster5', 'exhibition']</t>
+  </si>
+  <si>
+    <t>1f85673a-ba18-4aaf-821a-baf56c7efea7</t>
+  </si>
+  <si>
+    <t>90ebf3e8-d8ee-4b3b-9e62-3a17130bf3bf</t>
+  </si>
+  <si>
+    <t>aa8279d3-78cf-4af8-8f83-24dd44caabd6</t>
+  </si>
+  <si>
+    <t>elxsivkfcn</t>
+  </si>
+  <si>
+    <t>['lecture', 'culture', 'gardens']</t>
+  </si>
+  <si>
+    <t>3caa2392-510f-4c85-a489-b83e8200ff90</t>
+  </si>
+  <si>
+    <t>ddc06b8b-9dd1-4768-be15-75477b0f104a</t>
+  </si>
+  <si>
+    <t>55cdb198-f29d-466f-a4d9-a3a5dc9a3ec5</t>
+  </si>
+  <si>
+    <t>505d548a-6b67-416a-b85a-15dee47e855b</t>
+  </si>
+  <si>
+    <t>97dca6c1-6b1a-4ffe-a048-83ecce6707a5</t>
   </si>
   <si>
     <t>27b9e34f-c9da-47d5-a22e-d5140b9b0d18</t>
   </si>
   <si>
-    <t>f57a988c-883e-4f75-8dc6-7d5f76d005e5</t>
-  </si>
-  <si>
-    <t>43342fe3-e57f-4b74-883f-207d1cf0a24b</t>
-  </si>
-  <si>
-    <t>f61643e5-0237-4536-90ef-d3e8f721de21</t>
-  </si>
-  <si>
-    <t>krjyqnzsbl</t>
-  </si>
-  <si>
-    <t>['cluster5', 'architectonic', 'lecture']</t>
+    <t>0d9b11c5-4842-4d97-b105-908bca7c8fa5</t>
+  </si>
+  <si>
+    <t>qhrlazecip</t>
+  </si>
+  <si>
+    <t>['visual', 'castles', 'cluster2']</t>
+  </si>
+  <si>
+    <t>b0654f59-55d5-4c74-8420-3d3938f861e2</t>
+  </si>
+  <si>
+    <t>jzcgoxqrbu</t>
+  </si>
+  <si>
+    <t>['library', 'gardens']</t>
+  </si>
+  <si>
+    <t>3dc8fd2b-b27d-4552-8e95-7b51c95c08c9</t>
+  </si>
+  <si>
+    <t>43ae1a05-2981-4201-8c97-19a696eb0c5e</t>
+  </si>
+  <si>
+    <t>38609b0d-35a3-43ce-9896-d7c42996b702</t>
+  </si>
+  <si>
+    <t>51f2f922-3ec1-4a76-aa53-703e88dd7056</t>
+  </si>
+  <si>
+    <t>683844c9-9eb9-4adc-9f21-910cbeebe9dc</t>
+  </si>
+  <si>
+    <t>10f92ca9-be97-40d2-b2ad-cb99d5154981</t>
+  </si>
+  <si>
+    <t>c4ec2b8c-2aef-4e26-893a-ead4f7703e53</t>
+  </si>
+  <si>
+    <t>1259b27a-48fb-48d4-adbb-31329be57921</t>
+  </si>
+  <si>
+    <t>mqorxzhnfl</t>
+  </si>
+  <si>
+    <t>['cluster2', 'gardens', 'exhibition']</t>
+  </si>
+  <si>
+    <t>jbwsyquaox</t>
+  </si>
+  <si>
+    <t>['gardens', 'cluster3', 'architectonic']</t>
+  </si>
+  <si>
+    <t>80d22ad4-79ea-4688-97ec-4c93dc366e48</t>
+  </si>
+  <si>
+    <t>e89e2757-e3e7-4d22-bba5-58f4164a0105</t>
+  </si>
+  <si>
+    <t>fhcozyikgx</t>
+  </si>
+  <si>
+    <t>['military', 'exhibition']</t>
+  </si>
+  <si>
+    <t>4c123cbb-afaa-4150-94ff-4b94dfc60b4f</t>
+  </si>
+  <si>
+    <t>b67b0651-df2f-48c8-9793-1024a0c9901e</t>
+  </si>
+  <si>
+    <t>rqfuydwano</t>
+  </si>
+  <si>
+    <t>['cluster5', 'lecture']</t>
   </si>
   <si>
     <t>c40020e4-d23b-4607-9145-7aa020866c04</t>
   </si>
   <si>
-    <t>jqlckxnreu</t>
-  </si>
-  <si>
-    <t>['architectonic', 'gardens', 'library']</t>
-  </si>
-  <si>
-    <t>c4cc477e-1442-4ef9-96ea-539e46356b07</t>
-  </si>
-  <si>
-    <t>ef3c203e-a858-4f66-b2c8-59793913a386</t>
-  </si>
-  <si>
-    <t>1335f2de-05b0-4351-8cae-1cb1263b3791</t>
-  </si>
-  <si>
-    <t>7a2966b5-97fa-4cd3-9408-9e415182ca4e</t>
-  </si>
-  <si>
-    <t>fb32cee8-c9ce-47fa-b7f0-1d0b814b759e</t>
-  </si>
-  <si>
-    <t>19c6eb6a-fbd4-4bf3-a55c-72dd68d0fbe8</t>
-  </si>
-  <si>
-    <t>b5f1962b-3709-4476-a8c7-6209ca198c7d</t>
-  </si>
-  <si>
-    <t>41a0a29c-a655-4f51-979c-7fa624b303ea</t>
-  </si>
-  <si>
-    <t>00965172-fde6-42f1-8dae-116cae5ec572</t>
-  </si>
-  <si>
-    <t>682197a8-0359-4094-8281-ffa059de480f</t>
-  </si>
-  <si>
-    <t>feqszgunji</t>
-  </si>
-  <si>
-    <t>['cluster8', 'cluster2', 'parking']</t>
-  </si>
-  <si>
-    <t>044424ba-e4e7-4de8-b88c-ccaf14cf4c59</t>
-  </si>
-  <si>
-    <t>qneajrzymv</t>
-  </si>
-  <si>
-    <t>['cluster3', 'historic_location', 'library']</t>
-  </si>
-  <si>
-    <t>d1e42c4d-d176-4833-98a8-a3fb4a725b91</t>
-  </si>
-  <si>
-    <t>hdxpefyvgc</t>
-  </si>
-  <si>
-    <t>['parking', 'architectonic', 'cluster3']</t>
-  </si>
-  <si>
-    <t>832cd1d6-c933-4279-8ae6-1e3fa38853a2</t>
-  </si>
-  <si>
-    <t>e89e2757-e3e7-4d22-bba5-58f4164a0105</t>
-  </si>
-  <si>
-    <t>vsqwnurcog</t>
-  </si>
-  <si>
-    <t>['library', 'cluster0', 'naval']</t>
-  </si>
-  <si>
-    <t>d280a91d-ebc1-4607-afb9-e38a67c862d0</t>
-  </si>
-  <si>
-    <t>nagkxleity</t>
-  </si>
-  <si>
-    <t>['cluster3', 'nature', 'exhibition']</t>
-  </si>
-  <si>
-    <t>af698204-4437-411f-a1a9-d5a0fe7d16bb</t>
-  </si>
-  <si>
-    <t>aredwuqsjo</t>
-  </si>
-  <si>
-    <t>['cluster6', 'audiotour', 'architectonic']</t>
-  </si>
-  <si>
-    <t>424e8423-e43b-48e8-ad19-821014020860</t>
+    <t>d545be8a-48d2-4af9-862d-d26a821787e0</t>
   </si>
 </sst>
 </file>
@@ -524,7 +533,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -561,29 +570,73 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -610,16 +663,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -627,9 +680,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -654,16 +707,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -671,16 +724,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -688,33 +741,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -722,9 +758,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -749,60 +785,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
         <v>17</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -810,16 +802,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -827,16 +819,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
         <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -844,16 +836,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -861,16 +853,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -878,16 +870,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -895,16 +887,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -912,50 +904,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -990,16 +948,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1008,6 +966,169 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1034,16 +1155,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1051,7 +1172,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -1078,16 +1199,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1095,16 +1216,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1112,9 +1233,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1139,60 +1260,33 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
         <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed import files (museum_final.csv)
</commit_message>
<xml_diff>
--- a/input_excel.xlsx
+++ b/input_excel.xlsx
@@ -7,23 +7,23 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="txqwemihbl" sheetId="1" r:id="rId1"/>
-    <sheet name="nzwatlvupy" sheetId="2" r:id="rId2"/>
-    <sheet name="cftpkxgnrv" sheetId="3" r:id="rId3"/>
-    <sheet name="adswqujizy" sheetId="4" r:id="rId4"/>
-    <sheet name="oxhvybtnsw" sheetId="5" r:id="rId5"/>
-    <sheet name="ushdbgfvpl" sheetId="6" r:id="rId6"/>
-    <sheet name="upnxeodzsv" sheetId="7" r:id="rId7"/>
-    <sheet name="wqobvrsieu" sheetId="8" r:id="rId8"/>
-    <sheet name="puhcofwbya" sheetId="9" r:id="rId9"/>
-    <sheet name="xgubcwtiel" sheetId="10" r:id="rId10"/>
+    <sheet name="gjesufoblw" sheetId="1" r:id="rId1"/>
+    <sheet name="bmrktqyaih" sheetId="2" r:id="rId2"/>
+    <sheet name="fbetnhlvgu" sheetId="3" r:id="rId3"/>
+    <sheet name="vztngrocjb" sheetId="4" r:id="rId4"/>
+    <sheet name="hixypgktaz" sheetId="5" r:id="rId5"/>
+    <sheet name="vjckxtnyuq" sheetId="6" r:id="rId6"/>
+    <sheet name="tgywjsxkpa" sheetId="7" r:id="rId7"/>
+    <sheet name="qifnjkgemh" sheetId="8" r:id="rId8"/>
+    <sheet name="zamwdtokil" sheetId="9" r:id="rId9"/>
+    <sheet name="dxamzycpqf" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="93">
   <si>
     <t>clientid</t>
   </si>
@@ -37,274 +37,271 @@
     <t>museum_name</t>
   </si>
   <si>
-    <t>txqwemihbl</t>
-  </si>
-  <si>
-    <t>['castles']</t>
-  </si>
-  <si>
-    <t>Kasteel Hoensbroek</t>
-  </si>
-  <si>
-    <t>Kasteel Keukenhof</t>
-  </si>
-  <si>
-    <t>Kasteel Amerongen</t>
-  </si>
-  <si>
-    <t>Kasteel Huis Bergh</t>
-  </si>
-  <si>
-    <t>Kasteel Cannenburch</t>
-  </si>
-  <si>
-    <t>Kasteel Doornenburg</t>
-  </si>
-  <si>
-    <t>nzwatlvupy</t>
-  </si>
-  <si>
-    <t>['naval']</t>
-  </si>
-  <si>
-    <t>Museum In 't Houten Huis</t>
-  </si>
-  <si>
-    <t>Rijksmuseum Amsterdam</t>
+    <t>gjesufoblw</t>
+  </si>
+  <si>
+    <t>['cluster6']</t>
+  </si>
+  <si>
+    <t>Museumpark Archeon</t>
+  </si>
+  <si>
+    <t>Miramar Zeemuseum</t>
+  </si>
+  <si>
+    <t>Museum 'De Tien Malen'</t>
+  </si>
+  <si>
+    <t>Gemeentelijk Archeologisch Museum Aardenburg</t>
+  </si>
+  <si>
+    <t>Industrieel Museum Zeeland</t>
+  </si>
+  <si>
+    <t>De Koperen Knop</t>
+  </si>
+  <si>
+    <t>Oudheidkamer Texel</t>
+  </si>
+  <si>
+    <t>Flipje en Streekmuseum Tiel</t>
+  </si>
+  <si>
+    <t>Drents Museum</t>
+  </si>
+  <si>
+    <t>Natuurhistorisch Museum Maastricht</t>
+  </si>
+  <si>
+    <t>bmrktqyaih</t>
+  </si>
+  <si>
+    <t>['children']</t>
+  </si>
+  <si>
+    <t>Brabants Museum Oud Oosterhout</t>
+  </si>
+  <si>
+    <t>Natuurmuseum Fryslân</t>
+  </si>
+  <si>
+    <t>Zeeuws Maritiem MuZEEum</t>
+  </si>
+  <si>
+    <t>PreHistorisch Dorp</t>
+  </si>
+  <si>
+    <t>NEMO Science Museum</t>
+  </si>
+  <si>
+    <t>Veiligheidsmuseum PIT</t>
+  </si>
+  <si>
+    <t>fbetnhlvgu</t>
+  </si>
+  <si>
+    <t>['restaurant']</t>
+  </si>
+  <si>
+    <t>Museum Weesp</t>
+  </si>
+  <si>
+    <t>Interactief Museum Sow to Grow</t>
+  </si>
+  <si>
+    <t>mij | museum ijsselstein</t>
+  </si>
+  <si>
+    <t>Museum De Zwarte Tulp</t>
+  </si>
+  <si>
+    <t>Graafs Museum</t>
+  </si>
+  <si>
+    <t>Museum Catharijneconvent</t>
+  </si>
+  <si>
+    <t>Museum van Bommel van Dam</t>
+  </si>
+  <si>
+    <t>Louwman Museum</t>
+  </si>
+  <si>
+    <t>MU</t>
+  </si>
+  <si>
+    <t>Portrait Gallery of the 17th Century</t>
+  </si>
+  <si>
+    <t>vztngrocjb</t>
+  </si>
+  <si>
+    <t>['military']</t>
+  </si>
+  <si>
+    <t>Oorlogsmuseum Overloon</t>
+  </si>
+  <si>
+    <t>Geniemuseum</t>
   </si>
   <si>
     <t>Marinemuseum</t>
   </si>
   <si>
-    <t>Zuiderzeemuseum</t>
-  </si>
-  <si>
-    <t>Mariniersmuseum</t>
-  </si>
-  <si>
-    <t>Nationaal Sleepvaart Museum</t>
-  </si>
-  <si>
-    <t>Veenkoloniaal Museum</t>
-  </si>
-  <si>
-    <t>Biesbosch MuseumEiland</t>
-  </si>
-  <si>
-    <t>Het Scheepvaartmuseum</t>
-  </si>
-  <si>
-    <t>cftpkxgnrv</t>
+    <t>hixypgktaz</t>
   </si>
   <si>
     <t>['trainstation']</t>
   </si>
   <si>
-    <t>Villa Mondriaan</t>
-  </si>
-  <si>
-    <t>Vechtstreekmuseum</t>
+    <t>Honig Breethuis</t>
+  </si>
+  <si>
+    <t>Stedelijk Museum Alkmaar</t>
+  </si>
+  <si>
+    <t>Comenius Museum</t>
+  </si>
+  <si>
+    <t>Stedelijk Museum Amsterdam</t>
+  </si>
+  <si>
+    <t>Universiteitsmuseum Groningen</t>
+  </si>
+  <si>
+    <t>Museum de Kantfabriek</t>
   </si>
   <si>
     <t>Koninklijk Paleis Amsterdam</t>
   </si>
   <si>
-    <t>Nationaal Onderduikmuseum</t>
-  </si>
-  <si>
-    <t>Comenius Museum</t>
-  </si>
-  <si>
-    <t>Joods Historisch Museum</t>
-  </si>
-  <si>
-    <t>adswqujizy</t>
-  </si>
-  <si>
-    <t>['art_museum']</t>
-  </si>
-  <si>
-    <t>Museum Wierdenland Ezinge</t>
-  </si>
-  <si>
-    <t>Gorcums Museum</t>
-  </si>
-  <si>
-    <t>Grachtenmuseum Amsterdam</t>
-  </si>
-  <si>
-    <t>Museum de Buitenplaats</t>
-  </si>
-  <si>
-    <t>Museum De Lakenhal</t>
-  </si>
-  <si>
-    <t>Museum Slager</t>
-  </si>
-  <si>
-    <t>Museum van Bommel van Dam</t>
-  </si>
-  <si>
-    <t>Rijksmuseum van Oudheden</t>
-  </si>
-  <si>
-    <t>Anton Pieck Museum</t>
-  </si>
-  <si>
-    <t>De Mesdag Collectie</t>
-  </si>
-  <si>
-    <t>oxhvybtnsw</t>
-  </si>
-  <si>
-    <t>Stedelijk Museum Amsterdam</t>
-  </si>
-  <si>
-    <t>Kunsthal  Rotterdam</t>
-  </si>
-  <si>
-    <t>Stedelijk Museum Alkmaar</t>
+    <t>vjckxtnyuq</t>
+  </si>
+  <si>
+    <t>Nationaal Onderwijsmuseum</t>
+  </si>
+  <si>
+    <t>Museum 't Behouden Huys</t>
+  </si>
+  <si>
+    <t>Museum Het Pakhuis</t>
+  </si>
+  <si>
+    <t>Museum Tromp's Huys</t>
+  </si>
+  <si>
+    <t>De Bastei</t>
+  </si>
+  <si>
+    <t>tgywjsxkpa</t>
+  </si>
+  <si>
+    <t>['parking']</t>
+  </si>
+  <si>
+    <t>Feyenoord Museum</t>
+  </si>
+  <si>
+    <t>Trompenburg Tuinen &amp; Arboretum</t>
+  </si>
+  <si>
+    <t>Het Nederlands Vestingmuseum</t>
+  </si>
+  <si>
+    <t>Historische Tuin Aalsmeer</t>
+  </si>
+  <si>
+    <t>Openluchtmuseum en Themapark De Spitkeet</t>
+  </si>
+  <si>
+    <t>Openluchtmuseum Ootmarsum</t>
+  </si>
+  <si>
+    <t>qifnjkgemh</t>
+  </si>
+  <si>
+    <t>ABC Architectuurcentrum Haarlem</t>
+  </si>
+  <si>
+    <t>Museum Hindeloopen</t>
+  </si>
+  <si>
+    <t>Museum het Petershuis</t>
+  </si>
+  <si>
+    <t>Betje Wolff Museum</t>
+  </si>
+  <si>
+    <t>Museum Gevangenpoort</t>
+  </si>
+  <si>
+    <t>Rijssens Museum</t>
+  </si>
+  <si>
+    <t>Missiemuseum Steyl</t>
+  </si>
+  <si>
+    <t>De Glasblazerij</t>
+  </si>
+  <si>
+    <t>Museum Nairac</t>
+  </si>
+  <si>
+    <t>zamwdtokil</t>
+  </si>
+  <si>
+    <t>['library']</t>
+  </si>
+  <si>
+    <t>Foam Fotografiemuseum Amsterdam</t>
+  </si>
+  <si>
+    <t>Heerenveen Museum</t>
+  </si>
+  <si>
+    <t>Zaans Museum</t>
+  </si>
+  <si>
+    <t>Natuurhistorisch Museum Rotterdam</t>
   </si>
   <si>
     <t>Museum Gouda</t>
   </si>
   <si>
-    <t>Formerly known as Witte de With Center for Contemporary Art</t>
-  </si>
-  <si>
-    <t>Vincent van GoghHuis</t>
-  </si>
-  <si>
-    <t>Museum Helmond</t>
-  </si>
-  <si>
-    <t>ushdbgfvpl</t>
-  </si>
-  <si>
-    <t>['cluster0']</t>
-  </si>
-  <si>
-    <t>Museum Het Valkhof</t>
-  </si>
-  <si>
-    <t>Westlands Museum</t>
-  </si>
-  <si>
-    <t>Huis Van Gijn</t>
-  </si>
-  <si>
-    <t>Anne Frank Huis</t>
-  </si>
-  <si>
-    <t>Vrijheidsmuseum</t>
-  </si>
-  <si>
-    <t>Westfries Museum</t>
-  </si>
-  <si>
-    <t>Museum Drachten</t>
-  </si>
-  <si>
-    <t>Fries Verzetsmuseum</t>
-  </si>
-  <si>
-    <t>Het Noordbrabants Museum</t>
-  </si>
-  <si>
-    <t>upnxeodzsv</t>
-  </si>
-  <si>
-    <t>['military']</t>
-  </si>
-  <si>
-    <t>Oorlogsmuseum Overloon</t>
-  </si>
-  <si>
-    <t>Geniemuseum</t>
-  </si>
-  <si>
-    <t>wqobvrsieu</t>
-  </si>
-  <si>
-    <t>['cluster9']</t>
-  </si>
-  <si>
-    <t>Zwanenbroedershuis</t>
-  </si>
-  <si>
-    <t>Nederlands Zouavenmuseum</t>
-  </si>
-  <si>
-    <t>De Halve Maen</t>
-  </si>
-  <si>
-    <t>Frans Hals Museum Hof</t>
+    <t>Groninger Museum</t>
+  </si>
+  <si>
+    <t>Nederlands Zilvermuseum</t>
+  </si>
+  <si>
+    <t>dxamzycpqf</t>
+  </si>
+  <si>
+    <t>['historic_museum']</t>
+  </si>
+  <si>
+    <t>Museum Dorestad</t>
+  </si>
+  <si>
+    <t>Historisch Museum Den Briel</t>
+  </si>
+  <si>
+    <t>Huizer Museum</t>
+  </si>
+  <si>
+    <t>Landbouw-Juttersmuseum 'Swartwoude'</t>
+  </si>
+  <si>
+    <t>Nationaal Holocaust Museum</t>
+  </si>
+  <si>
+    <t>NEST</t>
+  </si>
+  <si>
+    <t>Nationaal Tinnen Figuren Museum</t>
   </si>
   <si>
     <t>Heiligenbeeldenmuseum</t>
-  </si>
-  <si>
-    <t>Molenmuseum De Valk</t>
-  </si>
-  <si>
-    <t>Het Spinozahuis</t>
-  </si>
-  <si>
-    <t>Frans Hals Museum Hal</t>
-  </si>
-  <si>
-    <t>Van Gogh Museum</t>
-  </si>
-  <si>
-    <t>puhcofwbya</t>
-  </si>
-  <si>
-    <t>['library']</t>
-  </si>
-  <si>
-    <t>Zeeuws Maritiem MuZEEum</t>
-  </si>
-  <si>
-    <t>Museum De Wieger</t>
-  </si>
-  <si>
-    <t>Museum Rotterdam</t>
-  </si>
-  <si>
-    <t>Drents Museum</t>
-  </si>
-  <si>
-    <t>Nederlands Watermuseum</t>
-  </si>
-  <si>
-    <t>Museum Kaap Skil</t>
-  </si>
-  <si>
-    <t>Heerenveen Museum</t>
-  </si>
-  <si>
-    <t>Limburgs Museum</t>
-  </si>
-  <si>
-    <t>Keramiekmuseum Princessehof</t>
-  </si>
-  <si>
-    <t>xgubcwtiel</t>
-  </si>
-  <si>
-    <t>GeoFort</t>
-  </si>
-  <si>
-    <t>Nationaal Gevangenismuseum</t>
-  </si>
-  <si>
-    <t>Kasteel Rosendael</t>
-  </si>
-  <si>
-    <t>Natuurhistorisch Museum Rotterdam</t>
-  </si>
-  <si>
-    <t>Hortus Botanicus Leiden</t>
   </si>
 </sst>
 </file>
@@ -662,7 +659,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -782,6 +779,74 @@
       </c>
       <c r="E7" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -816,16 +881,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -833,16 +898,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -850,16 +915,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E4" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -867,16 +932,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -884,16 +949,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" t="s">
         <v>88</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -901,16 +966,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E7" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -918,16 +983,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -935,16 +1000,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -952,16 +1017,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -970,186 +1035,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -1176,16 +1061,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1193,16 +1078,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1210,16 +1095,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1227,16 +1112,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1244,16 +1129,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1261,16 +1146,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1278,16 +1163,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
         <v>23</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1295,7 +1180,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -1322,16 +1207,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1339,16 +1224,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1356,16 +1241,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1373,16 +1258,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1390,16 +1275,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1407,16 +1292,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
         <v>31</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1424,16 +1309,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
       <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
         <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1441,16 +1326,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1458,16 +1343,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1475,16 +1360,94 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1519,16 +1482,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
         <v>43</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1536,16 +1499,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1553,16 +1516,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1570,16 +1533,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1587,16 +1550,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1604,16 +1567,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1621,16 +1584,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1638,16 +1601,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1655,16 +1618,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1699,16 +1662,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
         <v>51</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1716,16 +1679,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1733,16 +1696,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1750,16 +1713,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
         <v>52</v>
-      </c>
-      <c r="E5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1767,16 +1730,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1784,16 +1747,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1801,16 +1764,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1818,16 +1781,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1835,16 +1798,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1854,7 +1817,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1879,16 +1842,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1896,16 +1859,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1913,16 +1876,101 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" t="s">
         <v>62</v>
       </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
         <v>63</v>
-      </c>
-      <c r="E4" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1932,7 +1980,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1957,16 +2005,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1974,16 +2022,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
         <v>66</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1991,16 +2039,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
         <v>67</v>
-      </c>
-      <c r="E4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2008,16 +2056,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2025,16 +2073,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2042,16 +2090,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2059,16 +2107,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2076,16 +2124,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2093,16 +2141,33 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2112,7 +2177,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2137,16 +2202,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2154,16 +2219,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" t="s">
         <v>77</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2171,16 +2236,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" t="s">
         <v>78</v>
-      </c>
-      <c r="E4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2188,16 +2253,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2205,16 +2270,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2222,16 +2287,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E7" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2239,16 +2304,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2256,33 +2321,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E10" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New demo scripts are added.
</commit_message>
<xml_diff>
--- a/input_excel.xlsx
+++ b/input_excel.xlsx
@@ -7,16 +7,29 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="zmqpilswfa" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="pmshxjcuzg" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="cvdyemfklt" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="frnvuokdbl" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="pgvluaczxy" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="mvgtkhqija" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="zpwkfdjxrb" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="vucdlyiphf" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="nbxrjzdmvy" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="wdnfmxurcl" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="puetfwkjng" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="krhpduxojn" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="awdqcsbyor" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="vixukgpzlo" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="ypdqrhmbls" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="vdhzwegspa" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="ktfgyjsqpm" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="pbxefwjhmc" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="jpkdtsmleb" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="dwlprxfhas" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="dgahcxwiyz" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="bmokcvtjui" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="wskmjepyql" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="gahvswyxec" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="euplftxnkv" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="dhsaqyobrp" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="qacltofrxh" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="tvyunkrhcx" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="kbyftzrvjm" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="cdebxrhivy" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="uldmhrokae" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="seyguqrdan" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="ohaswbvlnc" sheetId="23" state="visible" r:id="rId23"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -470,7 +483,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>zmqpilswfa</t>
+          <t>puetfwkjng</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -478,12 +491,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['cluster2']</t>
+          <t>['architectonic']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Kasteel Doornenburg</t>
+          <t>Storyworld | Forum Groningen</t>
         </is>
       </c>
     </row>
@@ -493,7 +506,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>zmqpilswfa</t>
+          <t>puetfwkjng</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -501,12 +514,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['cluster2']</t>
+          <t>['architectonic']</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Kasteel Rosendael</t>
+          <t>Huis Verwolde</t>
         </is>
       </c>
     </row>
@@ -516,7 +529,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>zmqpilswfa</t>
+          <t>puetfwkjng</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -524,12 +537,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['cluster2']</t>
+          <t>['architectonic']</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Kasteel Huis Bergh</t>
+          <t>Sint Jan Gouda</t>
         </is>
       </c>
     </row>
@@ -539,7 +552,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>zmqpilswfa</t>
+          <t>puetfwkjng</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -547,12 +560,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>['cluster2']</t>
+          <t>['architectonic']</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Museum Kasteel Wijchen</t>
+          <t>Stedelijk Museum Breda</t>
         </is>
       </c>
     </row>
@@ -603,7 +616,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>wdnfmxurcl</t>
+          <t>dwlprxfhas</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -611,12 +624,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['architectonic']</t>
+          <t>['audiotour']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Zwanenbroedershuis</t>
+          <t>Airborne Museum at Hartenstein</t>
         </is>
       </c>
     </row>
@@ -626,7 +639,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>wdnfmxurcl</t>
+          <t>dwlprxfhas</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -634,12 +647,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['architectonic']</t>
+          <t>['audiotour']</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Museum Menkemaborg</t>
+          <t>Rijksmuseum Muiderslot</t>
         </is>
       </c>
     </row>
@@ -649,7 +662,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>wdnfmxurcl</t>
+          <t>dwlprxfhas</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -657,12 +670,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['architectonic']</t>
+          <t>['audiotour']</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Portugese Synagoge Amsterdam</t>
+          <t>Koninklijk Paleis Amsterdam</t>
         </is>
       </c>
     </row>
@@ -672,7 +685,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>wdnfmxurcl</t>
+          <t>dwlprxfhas</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -680,12 +693,1140 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>['architectonic']</t>
+          <t>['audiotour']</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
+          <t>PreHistorisch Dorp</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>clientid</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>features</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>museum_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>dgahcxwiyz</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>['nature']</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Nederlands Watermuseum</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>dgahcxwiyz</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['nature']</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Openluchtmuseum de Locht</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>dgahcxwiyz</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>['nature']</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Miramar Zeemuseum</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>clientid</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>features</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>museum_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>bmokcvtjui</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>['local history war']</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Fotomuseum Den Haag</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>bmokcvtjui</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['local history war']</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Design Museum Den Bosch</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>bmokcvtjui</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>['local history war']</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Museum Hengelo</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>clientid</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>features</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>museum_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>wskmjepyql</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>['military']</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Geniemuseum</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>wskmjepyql</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['military']</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Marinemuseum</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>wskmjepyql</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>['military']</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Oorlogsmuseum Overloon</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>clientid</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>features</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>museum_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>gahvswyxec</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>['castles cluster']</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>De Mesdag Collectie</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>gahvswyxec</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['castles cluster']</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Trompenburg Tuinen &amp; Arboretum</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>gahvswyxec</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>['castles cluster']</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Pop Up Museum Oud Amelisweerd</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>gahvswyxec</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>['castles cluster']</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>De Oude Kerk</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>clientid</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>features</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>museum_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>euplftxnkv</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>['exhibition']</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>t Fiskershúske</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>euplftxnkv</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['exhibition']</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Heerenveen Museum</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>euplftxnkv</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>['exhibition']</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Beeld en Geluid Den Haag</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>euplftxnkv</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>['exhibition']</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Nederlands Volksbuurtmuseum</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>clientid</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>features</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>museum_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>dhsaqyobrp</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>['exhibition']</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Van Gogh Museum</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>dhsaqyobrp</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['exhibition']</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>De Fraeylemaborg</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>dhsaqyobrp</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>['exhibition']</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Museum van de 20e Eeuw</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>dhsaqyobrp</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>['exhibition']</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Museum Henriette Polak</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>clientid</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>features</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>museum_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>qacltofrxh</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>['trainstation']</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Limburgs Museum</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>qacltofrxh</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['trainstation']</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Museum Willet-Holthuysen</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>qacltofrxh</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>['trainstation']</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Veiligheidsmuseum PIT</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>qacltofrxh</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>['trainstation']</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Beeld en Geluid</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>clientid</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>features</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>museum_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>tvyunkrhcx</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>['culture']</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Streekmuseum Etten Leur</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>tvyunkrhcx</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['culture']</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Nationaal Onderduikmuseum</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>tvyunkrhcx</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>['culture']</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Spoorwegmuseum</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>tvyunkrhcx</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>['culture']</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>Storyworld | Forum Groningen</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>clientid</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>features</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>museum_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>kbyftzrvjm</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>['nature tech']</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Leudal Museum</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>kbyftzrvjm</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['nature tech']</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Museum Haarlem</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>kbyftzrvjm</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>['nature tech']</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Streekmuseum Schippersbeurs</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>kbyftzrvjm</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>['nature tech']</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Museumpark Archeon</t>
         </is>
       </c>
     </row>
@@ -736,7 +1877,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>pmshxjcuzg</t>
+          <t>krhpduxojn</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -744,12 +1885,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['cluster4']</t>
+          <t>['library']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Elisabeth Weeshuis Museum</t>
+          <t>DAF Museum</t>
         </is>
       </c>
     </row>
@@ -759,7 +1900,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>pmshxjcuzg</t>
+          <t>krhpduxojn</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -767,12 +1908,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['cluster4']</t>
+          <t>['library']</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Design Museum Den Bosch</t>
+          <t>Nationaal Reddingmuseum Dorus Rijkers</t>
         </is>
       </c>
     </row>
@@ -782,7 +1923,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>pmshxjcuzg</t>
+          <t>krhpduxojn</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -790,12 +1931,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['cluster4']</t>
+          <t>['library']</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Historisch Museum Den Briel</t>
+          <t>Libertum</t>
         </is>
       </c>
     </row>
@@ -805,7 +1946,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>pmshxjcuzg</t>
+          <t>krhpduxojn</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -813,12 +1954,544 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>['cluster4']</t>
+          <t>['library']</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Stadskasteel Zaltbommel</t>
+          <t>Museummolen en molenwinkel De Walvisch</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>clientid</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>features</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>museum_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>cdebxrhivy</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>['historical']</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Huygens' Hofwijck</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>cdebxrhivy</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['historical']</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Weegschaal Museum Naarden</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>cdebxrhivy</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>['historical']</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Museum Willet-Holthuysen</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>cdebxrhivy</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>['historical']</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Museum Ons' Lieve Heer op Solder</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>clientid</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>features</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>museum_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>uldmhrokae</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>['exhibitions artists']</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Anne Frank Huis</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>uldmhrokae</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['exhibitions artists']</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Venrays Museum</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>uldmhrokae</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>['exhibitions artists']</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Museum Martena</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>uldmhrokae</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>['exhibitions artists']</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Museum JAN</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>clientid</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>features</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>museum_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>seyguqrdan</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>['local history war']</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Fotomuseum Den Haag</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>seyguqrdan</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['local history war']</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Streekmuseum Stevensweert Ohé en Laak</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>seyguqrdan</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>['local history war']</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Elisabeth Weeshuis Museum</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>seyguqrdan</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>['local history war']</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Bakkerijmuseum De Oude Bakkerij</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>clientid</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>features</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>museum_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ohaswbvlnc</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>['castles cluster']</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Foam Fotografiemuseum Amsterdam</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ohaswbvlnc</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['castles cluster']</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Stadsmuseum Harderwijk</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ohaswbvlnc</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>['castles cluster']</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Vleeshal</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ohaswbvlnc</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>['castles cluster']</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>SCHUNCK</t>
         </is>
       </c>
     </row>
@@ -869,7 +2542,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>cvdyemfklt</t>
+          <t>awdqcsbyor</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -877,12 +2550,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['restaurant']</t>
+          <t>['castles cluster']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Beeld en Geluid Den Haag</t>
+          <t>Museum Swaensteyn</t>
         </is>
       </c>
     </row>
@@ -892,7 +2565,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>cvdyemfklt</t>
+          <t>awdqcsbyor</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -900,12 +2573,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['restaurant']</t>
+          <t>['castles cluster']</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Museum Catharijneconvent</t>
+          <t>TENT</t>
         </is>
       </c>
     </row>
@@ -915,7 +2588,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>cvdyemfklt</t>
+          <t>awdqcsbyor</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -923,12 +2596,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['restaurant']</t>
+          <t>['castles cluster']</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Tropenmuseum</t>
+          <t>Kranenburgh</t>
         </is>
       </c>
     </row>
@@ -938,7 +2611,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>cvdyemfklt</t>
+          <t>awdqcsbyor</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -946,12 +2619,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>['restaurant']</t>
+          <t>['castles cluster']</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Museum Nienoord, Borg en Nationaal Rijtuigmuseum</t>
+          <t>Buitenplaats Kasteel Wijlre</t>
         </is>
       </c>
     </row>
@@ -961,6 +2634,116 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>clientid</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>features</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>museum_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>vixukgpzlo</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>['visual historical art']</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Gelders Geologisch Museum</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>vixukgpzlo</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['visual historical art']</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Observeum Burgum</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>vixukgpzlo</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>['visual historical art']</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Stadsmuseum Rhenen</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1002,7 +2785,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>frnvuokdbl</t>
+          <t>ypdqrhmbls</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1010,12 +2793,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['cluster5']</t>
+          <t>['historical']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Tongerlohuys</t>
+          <t>Diamant Museum Amsterdam</t>
         </is>
       </c>
     </row>
@@ -1025,7 +2808,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>frnvuokdbl</t>
+          <t>ypdqrhmbls</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -1033,12 +2816,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['cluster5']</t>
+          <t>['historical']</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Nederlands Tegelmuseum</t>
+          <t>Paleis Het Loo</t>
         </is>
       </c>
     </row>
@@ -1048,7 +2831,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>frnvuokdbl</t>
+          <t>ypdqrhmbls</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -1056,12 +2839,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['cluster5']</t>
+          <t>['historical']</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Spoorwegmuseum</t>
+          <t>Museum Paulina Bisdom van Vliet</t>
         </is>
       </c>
     </row>
@@ -1071,7 +2854,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>frnvuokdbl</t>
+          <t>ypdqrhmbls</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -1079,122 +2862,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>['cluster5']</t>
+          <t>['historical']</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Museum van de Vrouw</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>clientid</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>count</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>features</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>museum_name</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>pgvluaczxy</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>['educative']</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Openluchtmuseum en Themapark De Spitkeet</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>pgvluaczxy</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>['educative']</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>De Looierij</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>pgvluaczxy</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>['educative']</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Literatuurmuseum</t>
+          <t>Hermitage Amsterdam</t>
         </is>
       </c>
     </row>
@@ -1245,7 +2918,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>mvgtkhqija</t>
+          <t>vdhzwegspa</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1253,12 +2926,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['children']</t>
+          <t>['library']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Zeeuws Maritiem MuZEEum</t>
+          <t>Storyworld | Forum Groningen</t>
         </is>
       </c>
     </row>
@@ -1268,7 +2941,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>mvgtkhqija</t>
+          <t>vdhzwegspa</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -1276,12 +2949,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['children']</t>
+          <t>['library']</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Museum Speelklok</t>
+          <t>Museum Catharijneconvent</t>
         </is>
       </c>
     </row>
@@ -1291,7 +2964,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>mvgtkhqija</t>
+          <t>vdhzwegspa</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -1299,12 +2972,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['children']</t>
+          <t>['library']</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Belasting &amp; Douane Museum</t>
+          <t>Continium discovery center</t>
         </is>
       </c>
     </row>
@@ -1314,7 +2987,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>mvgtkhqija</t>
+          <t>vdhzwegspa</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -1322,12 +2995,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>['children']</t>
+          <t>['library']</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Museumpark Archeon</t>
+          <t>Natuurcentrum Ameland</t>
         </is>
       </c>
     </row>
@@ -1342,7 +3015,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1378,7 +3051,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>zpwkfdjxrb</t>
+          <t>ktfgyjsqpm</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1386,12 +3059,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['restaurant']</t>
+          <t>['art_galleries']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Van Gogh Museum</t>
+          <t>Marres, Huis voor Hedendaagse Kunst</t>
         </is>
       </c>
     </row>
@@ -1401,7 +3074,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>zpwkfdjxrb</t>
+          <t>ktfgyjsqpm</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -1409,35 +3082,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['restaurant']</t>
+          <t>['art_galleries']</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Design Museum Den Bosch</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>zpwkfdjxrb</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>['restaurant']</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Museum Kaap Skil</t>
+          <t>Het Nieuwe Instituut</t>
         </is>
       </c>
     </row>
@@ -1452,7 +3102,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1488,7 +3138,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>vucdlyiphf</t>
+          <t>pbxefwjhmc</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1496,12 +3146,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['cluster4']</t>
+          <t>['visual historical art']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Museum 't Behouden Huys</t>
+          <t>Biesbosch MuseumEiland</t>
         </is>
       </c>
     </row>
@@ -1511,7 +3161,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>vucdlyiphf</t>
+          <t>pbxefwjhmc</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -1519,12 +3169,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['cluster4']</t>
+          <t>['visual historical art']</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Fotomuseum Den Haag</t>
+          <t>Nationaal Sleepvaart Museum</t>
         </is>
       </c>
     </row>
@@ -1534,7 +3184,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>vucdlyiphf</t>
+          <t>pbxefwjhmc</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -1542,12 +3192,35 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['cluster4']</t>
+          <t>['visual historical art']</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Haags Historisch Museum</t>
+          <t>Streekmuseum Krimpenerwaard</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>pbxefwjhmc</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>['visual historical art']</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Oorlogsmuseum Overloon</t>
         </is>
       </c>
     </row>
@@ -1562,7 +3235,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1598,7 +3271,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>nbxrjzdmvy</t>
+          <t>jpkdtsmleb</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1606,12 +3279,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['cluster0']</t>
+          <t>['restaurant']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Museum Drachten</t>
+          <t>Foam Fotografiemuseum Amsterdam</t>
         </is>
       </c>
     </row>
@@ -1621,7 +3294,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>nbxrjzdmvy</t>
+          <t>jpkdtsmleb</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -1629,12 +3302,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['cluster0']</t>
+          <t>['restaurant']</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Purmerends Museum</t>
+          <t>Zaans Museum</t>
         </is>
       </c>
     </row>
@@ -1644,7 +3317,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>nbxrjzdmvy</t>
+          <t>jpkdtsmleb</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -1652,12 +3325,35 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['cluster0']</t>
+          <t>['restaurant']</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Museum Nijkerk</t>
+          <t>Museum Belvédère</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>jpkdtsmleb</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>['restaurant']</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Eye Filmmuseum</t>
         </is>
       </c>
     </row>

</xml_diff>